<commit_message>
Enabled back-projection of the adaptive remesher.
</commit_message>
<xml_diff>
--- a/MATLAB/analysis/volumeResults.xlsx
+++ b/MATLAB/analysis/volumeResults.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -10,17 +10,17 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46F37304-C368-4E60-82C1-4D3204F81B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990"/>
   </bookViews>
   <sheets>
     <sheet name="Volume" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" fullCalcOnLoad="true"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1046" uniqueCount="960">
   <si>
     <t>Bone name</t>
   </si>
@@ -443,6 +443,2454 @@
   </si>
   <si>
     <t>39 (5)</t>
+  </si>
+  <si>
+    <t>39 (4)</t>
+  </si>
+  <si>
+    <t>13 (1)</t>
+  </si>
+  <si>
+    <t>13 (2)</t>
+  </si>
+  <si>
+    <t>Sacrum</t>
+  </si>
+  <si>
+    <t>Hip_R</t>
+  </si>
+  <si>
+    <t>Hip_L</t>
+  </si>
+  <si>
+    <t>Femur_R</t>
+  </si>
+  <si>
+    <t>Femur_L</t>
+  </si>
+  <si>
+    <t>Patella_R</t>
+  </si>
+  <si>
+    <t>Patella_L</t>
+  </si>
+  <si>
+    <t>Tibia_R</t>
+  </si>
+  <si>
+    <t>Tibia_L</t>
+  </si>
+  <si>
+    <t>Fibula_R</t>
+  </si>
+  <si>
+    <t>Fibula_L</t>
+  </si>
+  <si>
+    <t>Talus_R</t>
+  </si>
+  <si>
+    <t>Talus_L</t>
+  </si>
+  <si>
+    <t>Calcaneus_R</t>
+  </si>
+  <si>
+    <t>Calcaneus_L</t>
+  </si>
+  <si>
+    <t>Tarsals_R</t>
+  </si>
+  <si>
+    <t>Tarsals_L</t>
+  </si>
+  <si>
+    <t>Metatarsals_R</t>
+  </si>
+  <si>
+    <t>Metatarsals_L</t>
+  </si>
+  <si>
+    <t>Phalanges_R</t>
+  </si>
+  <si>
+    <t>Phalanges_L</t>
+  </si>
+  <si>
+    <t>203 ± 27</t>
+  </si>
+  <si>
+    <t>327 ± 56</t>
+  </si>
+  <si>
+    <t>328 ± 55</t>
+  </si>
+  <si>
+    <t>531 ± 113</t>
+  </si>
+  <si>
+    <t>533 ± 113</t>
+  </si>
+  <si>
+    <t>19 ± 5</t>
+  </si>
+  <si>
+    <t>333 ± 74</t>
+  </si>
+  <si>
+    <t>336 ± 73</t>
+  </si>
+  <si>
+    <t>61 ± 16</t>
+  </si>
+  <si>
+    <t>60 ± 15</t>
+  </si>
+  <si>
+    <t>37 ± 9</t>
+  </si>
+  <si>
+    <t>38 ± 9</t>
+  </si>
+  <si>
+    <t>70 ± 14</t>
+  </si>
+  <si>
+    <t>43 ± 9</t>
+  </si>
+  <si>
+    <t>43 ± 10</t>
+  </si>
+  <si>
+    <t>48 ± 10</t>
+  </si>
+  <si>
+    <t>48 ± 9</t>
+  </si>
+  <si>
+    <t>15 ± 3</t>
+  </si>
+  <si>
+    <t>198 (35)</t>
+  </si>
+  <si>
+    <t>312 (90)</t>
+  </si>
+  <si>
+    <t>313 (91)</t>
+  </si>
+  <si>
+    <t>542 (214)</t>
+  </si>
+  <si>
+    <t>545 (209)</t>
+  </si>
+  <si>
+    <t>19 (7)</t>
+  </si>
+  <si>
+    <t>352 (135)</t>
+  </si>
+  <si>
+    <t>353 (139)</t>
+  </si>
+  <si>
+    <t>62 (21)</t>
+  </si>
+  <si>
+    <t>59 (20)</t>
+  </si>
+  <si>
+    <t>35 (17)</t>
+  </si>
+  <si>
+    <t>35 (16)</t>
+  </si>
+  <si>
+    <t>68 (24)</t>
+  </si>
+  <si>
+    <t>69 (22)</t>
+  </si>
+  <si>
+    <t>43 (16)</t>
+  </si>
+  <si>
+    <t>43 (17)</t>
+  </si>
+  <si>
+    <t>47 (17)</t>
+  </si>
+  <si>
+    <t>15 (5)</t>
+  </si>
+  <si>
+    <t>15 (4)</t>
+  </si>
+  <si>
+    <t>208 ± 27</t>
+  </si>
+  <si>
+    <t>365 ± 52</t>
+  </si>
+  <si>
+    <t>364 ± 50</t>
+  </si>
+  <si>
+    <t>624 ± 66</t>
+  </si>
+  <si>
+    <t>630 ± 57</t>
+  </si>
+  <si>
+    <t>23 ± 4</t>
+  </si>
+  <si>
+    <t>395 ± 39</t>
+  </si>
+  <si>
+    <t>398 ± 35</t>
+  </si>
+  <si>
+    <t>73 ± 12</t>
+  </si>
+  <si>
+    <t>70 ± 13</t>
+  </si>
+  <si>
+    <t>44 ± 6</t>
+  </si>
+  <si>
+    <t>80 ± 11</t>
+  </si>
+  <si>
+    <t>80 ± 10</t>
+  </si>
+  <si>
+    <t>50 ± 6</t>
+  </si>
+  <si>
+    <t>56 ± 6</t>
+  </si>
+  <si>
+    <t>56 ± 5</t>
+  </si>
+  <si>
+    <t>18 ± 3</t>
+  </si>
+  <si>
+    <t>215 (42)</t>
+  </si>
+  <si>
+    <t>382 (83)</t>
+  </si>
+  <si>
+    <t>381 (81)</t>
+  </si>
+  <si>
+    <t>630 (94)</t>
+  </si>
+  <si>
+    <t>631 (47)</t>
+  </si>
+  <si>
+    <t>21 (6)</t>
+  </si>
+  <si>
+    <t>22 (4)</t>
+  </si>
+  <si>
+    <t>394 (47)</t>
+  </si>
+  <si>
+    <t>402 (32)</t>
+  </si>
+  <si>
+    <t>69 (13)</t>
+  </si>
+  <si>
+    <t>66 (10)</t>
+  </si>
+  <si>
+    <t>46 (9)</t>
+  </si>
+  <si>
+    <t>44 (5)</t>
+  </si>
+  <si>
+    <t>80 (7)</t>
+  </si>
+  <si>
+    <t>81 (8)</t>
+  </si>
+  <si>
+    <t>49 (9)</t>
+  </si>
+  <si>
+    <t>50 (8)</t>
+  </si>
+  <si>
+    <t>56 (5)</t>
+  </si>
+  <si>
+    <t>55 (3)</t>
+  </si>
+  <si>
+    <t>17 (3)</t>
+  </si>
+  <si>
+    <t>17 (2)</t>
+  </si>
+  <si>
+    <t>198 ± 27</t>
+  </si>
+  <si>
+    <t>290 ± 28</t>
+  </si>
+  <si>
+    <t>292 ± 31</t>
+  </si>
+  <si>
+    <t>437 ± 56</t>
+  </si>
+  <si>
+    <t>436 ± 55</t>
+  </si>
+  <si>
+    <t>15 ± 2</t>
+  </si>
+  <si>
+    <t>15 ± 3</t>
+  </si>
+  <si>
+    <t>270 ± 37</t>
+  </si>
+  <si>
+    <t>274 ± 38</t>
+  </si>
+  <si>
+    <t>50 ± 8</t>
+  </si>
+  <si>
+    <t>50 ± 9</t>
+  </si>
+  <si>
+    <t>30 ± 5</t>
+  </si>
+  <si>
+    <t>31 ± 6</t>
+  </si>
+  <si>
+    <t>59 ± 8</t>
+  </si>
+  <si>
+    <t>59 ± 9</t>
+  </si>
+  <si>
+    <t>36 ± 6</t>
+  </si>
+  <si>
+    <t>36 ± 7</t>
+  </si>
+  <si>
+    <t>40 ± 4</t>
+  </si>
+  <si>
+    <t>13 ± 1</t>
+  </si>
+  <si>
+    <t>193 (29)</t>
+  </si>
+  <si>
+    <t>292 (39)</t>
+  </si>
+  <si>
+    <t>290 (50)</t>
+  </si>
+  <si>
+    <t>416 (59)</t>
+  </si>
+  <si>
+    <t>422 (64)</t>
+  </si>
+  <si>
+    <t>15 (3)</t>
+  </si>
+  <si>
+    <t>16 (3)</t>
+  </si>
+  <si>
+    <t>259 (41)</t>
+  </si>
+  <si>
+    <t>263 (39)</t>
+  </si>
+  <si>
+    <t>48 (12)</t>
+  </si>
+  <si>
+    <t>47 (12)</t>
+  </si>
+  <si>
+    <t>29 (5)</t>
+  </si>
+  <si>
+    <t>30 (4)</t>
+  </si>
+  <si>
+    <t>56 (11)</t>
+  </si>
+  <si>
+    <t>59 (13)</t>
+  </si>
+  <si>
+    <t>34 (7)</t>
+  </si>
+  <si>
+    <t>35 (6)</t>
+  </si>
+  <si>
+    <t>38 (5)</t>
+  </si>
+  <si>
+    <t>39 (4)</t>
+  </si>
+  <si>
+    <t>13 (1)</t>
+  </si>
+  <si>
+    <t>13 (2)</t>
+  </si>
+  <si>
+    <t>Sacrum</t>
+  </si>
+  <si>
+    <t>Hip_R</t>
+  </si>
+  <si>
+    <t>Hip_L</t>
+  </si>
+  <si>
+    <t>Femur_R</t>
+  </si>
+  <si>
+    <t>Femur_L</t>
+  </si>
+  <si>
+    <t>Patella_R</t>
+  </si>
+  <si>
+    <t>Patella_L</t>
+  </si>
+  <si>
+    <t>Tibia_R</t>
+  </si>
+  <si>
+    <t>Tibia_L</t>
+  </si>
+  <si>
+    <t>Fibula_R</t>
+  </si>
+  <si>
+    <t>Fibula_L</t>
+  </si>
+  <si>
+    <t>Talus_R</t>
+  </si>
+  <si>
+    <t>Talus_L</t>
+  </si>
+  <si>
+    <t>Calcaneus_R</t>
+  </si>
+  <si>
+    <t>Calcaneus_L</t>
+  </si>
+  <si>
+    <t>Tarsals_R</t>
+  </si>
+  <si>
+    <t>Tarsals_L</t>
+  </si>
+  <si>
+    <t>Metatarsals_R</t>
+  </si>
+  <si>
+    <t>Metatarsals_L</t>
+  </si>
+  <si>
+    <t>Phalanges_R</t>
+  </si>
+  <si>
+    <t>Phalanges_L</t>
+  </si>
+  <si>
+    <t>203 ± 27</t>
+  </si>
+  <si>
+    <t>327 ± 56</t>
+  </si>
+  <si>
+    <t>328 ± 55</t>
+  </si>
+  <si>
+    <t>531 ± 113</t>
+  </si>
+  <si>
+    <t>533 ± 113</t>
+  </si>
+  <si>
+    <t>19 ± 5</t>
+  </si>
+  <si>
+    <t>333 ± 74</t>
+  </si>
+  <si>
+    <t>336 ± 73</t>
+  </si>
+  <si>
+    <t>61 ± 16</t>
+  </si>
+  <si>
+    <t>60 ± 15</t>
+  </si>
+  <si>
+    <t>37 ± 9</t>
+  </si>
+  <si>
+    <t>38 ± 9</t>
+  </si>
+  <si>
+    <t>70 ± 14</t>
+  </si>
+  <si>
+    <t>43 ± 9</t>
+  </si>
+  <si>
+    <t>43 ± 10</t>
+  </si>
+  <si>
+    <t>48 ± 10</t>
+  </si>
+  <si>
+    <t>48 ± 9</t>
+  </si>
+  <si>
+    <t>15 ± 3</t>
+  </si>
+  <si>
+    <t>198 (35)</t>
+  </si>
+  <si>
+    <t>312 (90)</t>
+  </si>
+  <si>
+    <t>313 (91)</t>
+  </si>
+  <si>
+    <t>542 (214)</t>
+  </si>
+  <si>
+    <t>545 (209)</t>
+  </si>
+  <si>
+    <t>19 (7)</t>
+  </si>
+  <si>
+    <t>352 (135)</t>
+  </si>
+  <si>
+    <t>353 (139)</t>
+  </si>
+  <si>
+    <t>62 (21)</t>
+  </si>
+  <si>
+    <t>59 (20)</t>
+  </si>
+  <si>
+    <t>35 (17)</t>
+  </si>
+  <si>
+    <t>35 (16)</t>
+  </si>
+  <si>
+    <t>68 (24)</t>
+  </si>
+  <si>
+    <t>69 (22)</t>
+  </si>
+  <si>
+    <t>43 (16)</t>
+  </si>
+  <si>
+    <t>43 (17)</t>
+  </si>
+  <si>
+    <t>47 (17)</t>
+  </si>
+  <si>
+    <t>15 (5)</t>
+  </si>
+  <si>
+    <t>15 (4)</t>
+  </si>
+  <si>
+    <t>208 ± 27</t>
+  </si>
+  <si>
+    <t>365 ± 52</t>
+  </si>
+  <si>
+    <t>364 ± 50</t>
+  </si>
+  <si>
+    <t>624 ± 66</t>
+  </si>
+  <si>
+    <t>630 ± 57</t>
+  </si>
+  <si>
+    <t>23 ± 4</t>
+  </si>
+  <si>
+    <t>395 ± 39</t>
+  </si>
+  <si>
+    <t>398 ± 35</t>
+  </si>
+  <si>
+    <t>73 ± 12</t>
+  </si>
+  <si>
+    <t>70 ± 13</t>
+  </si>
+  <si>
+    <t>44 ± 6</t>
+  </si>
+  <si>
+    <t>80 ± 11</t>
+  </si>
+  <si>
+    <t>80 ± 10</t>
+  </si>
+  <si>
+    <t>50 ± 6</t>
+  </si>
+  <si>
+    <t>56 ± 6</t>
+  </si>
+  <si>
+    <t>56 ± 5</t>
+  </si>
+  <si>
+    <t>18 ± 3</t>
+  </si>
+  <si>
+    <t>215 (42)</t>
+  </si>
+  <si>
+    <t>382 (83)</t>
+  </si>
+  <si>
+    <t>381 (81)</t>
+  </si>
+  <si>
+    <t>630 (94)</t>
+  </si>
+  <si>
+    <t>631 (47)</t>
+  </si>
+  <si>
+    <t>21 (6)</t>
+  </si>
+  <si>
+    <t>22 (4)</t>
+  </si>
+  <si>
+    <t>394 (47)</t>
+  </si>
+  <si>
+    <t>402 (32)</t>
+  </si>
+  <si>
+    <t>69 (13)</t>
+  </si>
+  <si>
+    <t>66 (10)</t>
+  </si>
+  <si>
+    <t>46 (9)</t>
+  </si>
+  <si>
+    <t>44 (5)</t>
+  </si>
+  <si>
+    <t>80 (7)</t>
+  </si>
+  <si>
+    <t>81 (8)</t>
+  </si>
+  <si>
+    <t>49 (9)</t>
+  </si>
+  <si>
+    <t>50 (8)</t>
+  </si>
+  <si>
+    <t>56 (5)</t>
+  </si>
+  <si>
+    <t>55 (3)</t>
+  </si>
+  <si>
+    <t>17 (3)</t>
+  </si>
+  <si>
+    <t>17 (2)</t>
+  </si>
+  <si>
+    <t>198 ± 27</t>
+  </si>
+  <si>
+    <t>290 ± 28</t>
+  </si>
+  <si>
+    <t>292 ± 31</t>
+  </si>
+  <si>
+    <t>437 ± 56</t>
+  </si>
+  <si>
+    <t>436 ± 55</t>
+  </si>
+  <si>
+    <t>15 ± 2</t>
+  </si>
+  <si>
+    <t>15 ± 3</t>
+  </si>
+  <si>
+    <t>270 ± 37</t>
+  </si>
+  <si>
+    <t>274 ± 38</t>
+  </si>
+  <si>
+    <t>50 ± 8</t>
+  </si>
+  <si>
+    <t>50 ± 9</t>
+  </si>
+  <si>
+    <t>30 ± 5</t>
+  </si>
+  <si>
+    <t>31 ± 6</t>
+  </si>
+  <si>
+    <t>59 ± 8</t>
+  </si>
+  <si>
+    <t>59 ± 9</t>
+  </si>
+  <si>
+    <t>36 ± 6</t>
+  </si>
+  <si>
+    <t>36 ± 7</t>
+  </si>
+  <si>
+    <t>40 ± 4</t>
+  </si>
+  <si>
+    <t>13 ± 1</t>
+  </si>
+  <si>
+    <t>193 (29)</t>
+  </si>
+  <si>
+    <t>292 (39)</t>
+  </si>
+  <si>
+    <t>290 (50)</t>
+  </si>
+  <si>
+    <t>416 (59)</t>
+  </si>
+  <si>
+    <t>422 (64)</t>
+  </si>
+  <si>
+    <t>15 (3)</t>
+  </si>
+  <si>
+    <t>16 (3)</t>
+  </si>
+  <si>
+    <t>259 (41)</t>
+  </si>
+  <si>
+    <t>263 (39)</t>
+  </si>
+  <si>
+    <t>48 (12)</t>
+  </si>
+  <si>
+    <t>47 (12)</t>
+  </si>
+  <si>
+    <t>29 (5)</t>
+  </si>
+  <si>
+    <t>30 (4)</t>
+  </si>
+  <si>
+    <t>56 (11)</t>
+  </si>
+  <si>
+    <t>59 (13)</t>
+  </si>
+  <si>
+    <t>34 (7)</t>
+  </si>
+  <si>
+    <t>35 (6)</t>
+  </si>
+  <si>
+    <t>38 (5)</t>
+  </si>
+  <si>
+    <t>39 (4)</t>
+  </si>
+  <si>
+    <t>13 (1)</t>
+  </si>
+  <si>
+    <t>13 (2)</t>
+  </si>
+  <si>
+    <t>Sacrum</t>
+  </si>
+  <si>
+    <t>Hip_R</t>
+  </si>
+  <si>
+    <t>Hip_L</t>
+  </si>
+  <si>
+    <t>Femur_R</t>
+  </si>
+  <si>
+    <t>Femur_L</t>
+  </si>
+  <si>
+    <t>Patella_R</t>
+  </si>
+  <si>
+    <t>Patella_L</t>
+  </si>
+  <si>
+    <t>Tibia_R</t>
+  </si>
+  <si>
+    <t>Tibia_L</t>
+  </si>
+  <si>
+    <t>Fibula_R</t>
+  </si>
+  <si>
+    <t>Fibula_L</t>
+  </si>
+  <si>
+    <t>Talus_R</t>
+  </si>
+  <si>
+    <t>Talus_L</t>
+  </si>
+  <si>
+    <t>Calcaneus_R</t>
+  </si>
+  <si>
+    <t>Calcaneus_L</t>
+  </si>
+  <si>
+    <t>Tarsals_R</t>
+  </si>
+  <si>
+    <t>Tarsals_L</t>
+  </si>
+  <si>
+    <t>Metatarsals_R</t>
+  </si>
+  <si>
+    <t>Metatarsals_L</t>
+  </si>
+  <si>
+    <t>Phalanges_R</t>
+  </si>
+  <si>
+    <t>Phalanges_L</t>
+  </si>
+  <si>
+    <t>203 ± 27</t>
+  </si>
+  <si>
+    <t>327 ± 56</t>
+  </si>
+  <si>
+    <t>328 ± 55</t>
+  </si>
+  <si>
+    <t>531 ± 113</t>
+  </si>
+  <si>
+    <t>533 ± 113</t>
+  </si>
+  <si>
+    <t>19 ± 5</t>
+  </si>
+  <si>
+    <t>333 ± 74</t>
+  </si>
+  <si>
+    <t>336 ± 73</t>
+  </si>
+  <si>
+    <t>61 ± 16</t>
+  </si>
+  <si>
+    <t>60 ± 15</t>
+  </si>
+  <si>
+    <t>37 ± 9</t>
+  </si>
+  <si>
+    <t>38 ± 9</t>
+  </si>
+  <si>
+    <t>70 ± 14</t>
+  </si>
+  <si>
+    <t>43 ± 9</t>
+  </si>
+  <si>
+    <t>43 ± 10</t>
+  </si>
+  <si>
+    <t>48 ± 10</t>
+  </si>
+  <si>
+    <t>48 ± 9</t>
+  </si>
+  <si>
+    <t>15 ± 3</t>
+  </si>
+  <si>
+    <t>198 (35)</t>
+  </si>
+  <si>
+    <t>312 (90)</t>
+  </si>
+  <si>
+    <t>313 (91)</t>
+  </si>
+  <si>
+    <t>542 (214)</t>
+  </si>
+  <si>
+    <t>545 (209)</t>
+  </si>
+  <si>
+    <t>19 (7)</t>
+  </si>
+  <si>
+    <t>352 (135)</t>
+  </si>
+  <si>
+    <t>353 (139)</t>
+  </si>
+  <si>
+    <t>62 (21)</t>
+  </si>
+  <si>
+    <t>59 (20)</t>
+  </si>
+  <si>
+    <t>35 (17)</t>
+  </si>
+  <si>
+    <t>35 (16)</t>
+  </si>
+  <si>
+    <t>68 (24)</t>
+  </si>
+  <si>
+    <t>69 (22)</t>
+  </si>
+  <si>
+    <t>43 (16)</t>
+  </si>
+  <si>
+    <t>43 (17)</t>
+  </si>
+  <si>
+    <t>47 (17)</t>
+  </si>
+  <si>
+    <t>15 (5)</t>
+  </si>
+  <si>
+    <t>15 (4)</t>
+  </si>
+  <si>
+    <t>208 ± 27</t>
+  </si>
+  <si>
+    <t>365 ± 52</t>
+  </si>
+  <si>
+    <t>364 ± 50</t>
+  </si>
+  <si>
+    <t>624 ± 66</t>
+  </si>
+  <si>
+    <t>630 ± 57</t>
+  </si>
+  <si>
+    <t>23 ± 4</t>
+  </si>
+  <si>
+    <t>395 ± 39</t>
+  </si>
+  <si>
+    <t>398 ± 35</t>
+  </si>
+  <si>
+    <t>73 ± 12</t>
+  </si>
+  <si>
+    <t>70 ± 13</t>
+  </si>
+  <si>
+    <t>44 ± 6</t>
+  </si>
+  <si>
+    <t>80 ± 11</t>
+  </si>
+  <si>
+    <t>80 ± 10</t>
+  </si>
+  <si>
+    <t>50 ± 6</t>
+  </si>
+  <si>
+    <t>56 ± 6</t>
+  </si>
+  <si>
+    <t>56 ± 5</t>
+  </si>
+  <si>
+    <t>18 ± 3</t>
+  </si>
+  <si>
+    <t>215 (42)</t>
+  </si>
+  <si>
+    <t>382 (83)</t>
+  </si>
+  <si>
+    <t>381 (81)</t>
+  </si>
+  <si>
+    <t>630 (94)</t>
+  </si>
+  <si>
+    <t>631 (47)</t>
+  </si>
+  <si>
+    <t>21 (6)</t>
+  </si>
+  <si>
+    <t>22 (4)</t>
+  </si>
+  <si>
+    <t>394 (47)</t>
+  </si>
+  <si>
+    <t>402 (32)</t>
+  </si>
+  <si>
+    <t>69 (13)</t>
+  </si>
+  <si>
+    <t>66 (10)</t>
+  </si>
+  <si>
+    <t>46 (9)</t>
+  </si>
+  <si>
+    <t>44 (5)</t>
+  </si>
+  <si>
+    <t>80 (7)</t>
+  </si>
+  <si>
+    <t>81 (8)</t>
+  </si>
+  <si>
+    <t>49 (9)</t>
+  </si>
+  <si>
+    <t>50 (8)</t>
+  </si>
+  <si>
+    <t>56 (5)</t>
+  </si>
+  <si>
+    <t>55 (3)</t>
+  </si>
+  <si>
+    <t>17 (3)</t>
+  </si>
+  <si>
+    <t>17 (2)</t>
+  </si>
+  <si>
+    <t>198 ± 27</t>
+  </si>
+  <si>
+    <t>290 ± 28</t>
+  </si>
+  <si>
+    <t>292 ± 31</t>
+  </si>
+  <si>
+    <t>437 ± 56</t>
+  </si>
+  <si>
+    <t>436 ± 55</t>
+  </si>
+  <si>
+    <t>15 ± 2</t>
+  </si>
+  <si>
+    <t>15 ± 3</t>
+  </si>
+  <si>
+    <t>270 ± 37</t>
+  </si>
+  <si>
+    <t>274 ± 38</t>
+  </si>
+  <si>
+    <t>50 ± 8</t>
+  </si>
+  <si>
+    <t>50 ± 9</t>
+  </si>
+  <si>
+    <t>30 ± 5</t>
+  </si>
+  <si>
+    <t>31 ± 6</t>
+  </si>
+  <si>
+    <t>59 ± 8</t>
+  </si>
+  <si>
+    <t>59 ± 9</t>
+  </si>
+  <si>
+    <t>36 ± 6</t>
+  </si>
+  <si>
+    <t>36 ± 7</t>
+  </si>
+  <si>
+    <t>40 ± 4</t>
+  </si>
+  <si>
+    <t>13 ± 1</t>
+  </si>
+  <si>
+    <t>193 (29)</t>
+  </si>
+  <si>
+    <t>292 (39)</t>
+  </si>
+  <si>
+    <t>290 (50)</t>
+  </si>
+  <si>
+    <t>416 (59)</t>
+  </si>
+  <si>
+    <t>422 (64)</t>
+  </si>
+  <si>
+    <t>15 (3)</t>
+  </si>
+  <si>
+    <t>16 (3)</t>
+  </si>
+  <si>
+    <t>259 (41)</t>
+  </si>
+  <si>
+    <t>263 (39)</t>
+  </si>
+  <si>
+    <t>48 (12)</t>
+  </si>
+  <si>
+    <t>47 (12)</t>
+  </si>
+  <si>
+    <t>29 (5)</t>
+  </si>
+  <si>
+    <t>30 (4)</t>
+  </si>
+  <si>
+    <t>56 (11)</t>
+  </si>
+  <si>
+    <t>59 (13)</t>
+  </si>
+  <si>
+    <t>34 (7)</t>
+  </si>
+  <si>
+    <t>35 (6)</t>
+  </si>
+  <si>
+    <t>38 (5)</t>
+  </si>
+  <si>
+    <t>39 (4)</t>
+  </si>
+  <si>
+    <t>13 (1)</t>
+  </si>
+  <si>
+    <t>13 (2)</t>
+  </si>
+  <si>
+    <t>Sacrum</t>
+  </si>
+  <si>
+    <t>Hip_R</t>
+  </si>
+  <si>
+    <t>Hip_L</t>
+  </si>
+  <si>
+    <t>Femur_R</t>
+  </si>
+  <si>
+    <t>Femur_L</t>
+  </si>
+  <si>
+    <t>Patella_R</t>
+  </si>
+  <si>
+    <t>Patella_L</t>
+  </si>
+  <si>
+    <t>Tibia_R</t>
+  </si>
+  <si>
+    <t>Tibia_L</t>
+  </si>
+  <si>
+    <t>Fibula_R</t>
+  </si>
+  <si>
+    <t>Fibula_L</t>
+  </si>
+  <si>
+    <t>Talus_R</t>
+  </si>
+  <si>
+    <t>Talus_L</t>
+  </si>
+  <si>
+    <t>Calcaneus_R</t>
+  </si>
+  <si>
+    <t>Calcaneus_L</t>
+  </si>
+  <si>
+    <t>Tarsals_R</t>
+  </si>
+  <si>
+    <t>Tarsals_L</t>
+  </si>
+  <si>
+    <t>Metatarsals_R</t>
+  </si>
+  <si>
+    <t>Metatarsals_L</t>
+  </si>
+  <si>
+    <t>Phalanges_R</t>
+  </si>
+  <si>
+    <t>Phalanges_L</t>
+  </si>
+  <si>
+    <t>203 ± 27</t>
+  </si>
+  <si>
+    <t>327 ± 56</t>
+  </si>
+  <si>
+    <t>328 ± 55</t>
+  </si>
+  <si>
+    <t>531 ± 113</t>
+  </si>
+  <si>
+    <t>533 ± 113</t>
+  </si>
+  <si>
+    <t>19 ± 5</t>
+  </si>
+  <si>
+    <t>333 ± 74</t>
+  </si>
+  <si>
+    <t>336 ± 73</t>
+  </si>
+  <si>
+    <t>61 ± 16</t>
+  </si>
+  <si>
+    <t>60 ± 15</t>
+  </si>
+  <si>
+    <t>37 ± 9</t>
+  </si>
+  <si>
+    <t>38 ± 9</t>
+  </si>
+  <si>
+    <t>70 ± 14</t>
+  </si>
+  <si>
+    <t>43 ± 9</t>
+  </si>
+  <si>
+    <t>43 ± 10</t>
+  </si>
+  <si>
+    <t>48 ± 10</t>
+  </si>
+  <si>
+    <t>48 ± 9</t>
+  </si>
+  <si>
+    <t>15 ± 3</t>
+  </si>
+  <si>
+    <t>198 (35)</t>
+  </si>
+  <si>
+    <t>312 (90)</t>
+  </si>
+  <si>
+    <t>313 (91)</t>
+  </si>
+  <si>
+    <t>542 (214)</t>
+  </si>
+  <si>
+    <t>545 (209)</t>
+  </si>
+  <si>
+    <t>19 (7)</t>
+  </si>
+  <si>
+    <t>352 (135)</t>
+  </si>
+  <si>
+    <t>353 (139)</t>
+  </si>
+  <si>
+    <t>62 (21)</t>
+  </si>
+  <si>
+    <t>59 (20)</t>
+  </si>
+  <si>
+    <t>35 (17)</t>
+  </si>
+  <si>
+    <t>35 (16)</t>
+  </si>
+  <si>
+    <t>68 (24)</t>
+  </si>
+  <si>
+    <t>69 (22)</t>
+  </si>
+  <si>
+    <t>43 (16)</t>
+  </si>
+  <si>
+    <t>43 (17)</t>
+  </si>
+  <si>
+    <t>47 (17)</t>
+  </si>
+  <si>
+    <t>15 (5)</t>
+  </si>
+  <si>
+    <t>15 (4)</t>
+  </si>
+  <si>
+    <t>208 ± 27</t>
+  </si>
+  <si>
+    <t>365 ± 52</t>
+  </si>
+  <si>
+    <t>364 ± 50</t>
+  </si>
+  <si>
+    <t>624 ± 66</t>
+  </si>
+  <si>
+    <t>630 ± 57</t>
+  </si>
+  <si>
+    <t>23 ± 4</t>
+  </si>
+  <si>
+    <t>395 ± 39</t>
+  </si>
+  <si>
+    <t>398 ± 35</t>
+  </si>
+  <si>
+    <t>73 ± 12</t>
+  </si>
+  <si>
+    <t>70 ± 13</t>
+  </si>
+  <si>
+    <t>44 ± 6</t>
+  </si>
+  <si>
+    <t>80 ± 11</t>
+  </si>
+  <si>
+    <t>80 ± 10</t>
+  </si>
+  <si>
+    <t>50 ± 6</t>
+  </si>
+  <si>
+    <t>56 ± 6</t>
+  </si>
+  <si>
+    <t>56 ± 5</t>
+  </si>
+  <si>
+    <t>18 ± 3</t>
+  </si>
+  <si>
+    <t>215 (42)</t>
+  </si>
+  <si>
+    <t>382 (83)</t>
+  </si>
+  <si>
+    <t>381 (81)</t>
+  </si>
+  <si>
+    <t>630 (94)</t>
+  </si>
+  <si>
+    <t>631 (47)</t>
+  </si>
+  <si>
+    <t>21 (6)</t>
+  </si>
+  <si>
+    <t>22 (4)</t>
+  </si>
+  <si>
+    <t>394 (47)</t>
+  </si>
+  <si>
+    <t>402 (32)</t>
+  </si>
+  <si>
+    <t>69 (13)</t>
+  </si>
+  <si>
+    <t>66 (10)</t>
+  </si>
+  <si>
+    <t>46 (9)</t>
+  </si>
+  <si>
+    <t>44 (5)</t>
+  </si>
+  <si>
+    <t>80 (7)</t>
+  </si>
+  <si>
+    <t>81 (8)</t>
+  </si>
+  <si>
+    <t>49 (9)</t>
+  </si>
+  <si>
+    <t>50 (8)</t>
+  </si>
+  <si>
+    <t>56 (5)</t>
+  </si>
+  <si>
+    <t>55 (3)</t>
+  </si>
+  <si>
+    <t>17 (3)</t>
+  </si>
+  <si>
+    <t>17 (2)</t>
+  </si>
+  <si>
+    <t>198 ± 27</t>
+  </si>
+  <si>
+    <t>290 ± 28</t>
+  </si>
+  <si>
+    <t>292 ± 31</t>
+  </si>
+  <si>
+    <t>437 ± 56</t>
+  </si>
+  <si>
+    <t>436 ± 55</t>
+  </si>
+  <si>
+    <t>15 ± 2</t>
+  </si>
+  <si>
+    <t>15 ± 3</t>
+  </si>
+  <si>
+    <t>270 ± 37</t>
+  </si>
+  <si>
+    <t>274 ± 38</t>
+  </si>
+  <si>
+    <t>50 ± 8</t>
+  </si>
+  <si>
+    <t>50 ± 9</t>
+  </si>
+  <si>
+    <t>30 ± 5</t>
+  </si>
+  <si>
+    <t>31 ± 6</t>
+  </si>
+  <si>
+    <t>59 ± 8</t>
+  </si>
+  <si>
+    <t>59 ± 9</t>
+  </si>
+  <si>
+    <t>36 ± 6</t>
+  </si>
+  <si>
+    <t>36 ± 7</t>
+  </si>
+  <si>
+    <t>40 ± 4</t>
+  </si>
+  <si>
+    <t>13 ± 1</t>
+  </si>
+  <si>
+    <t>193 (29)</t>
+  </si>
+  <si>
+    <t>292 (39)</t>
+  </si>
+  <si>
+    <t>290 (50)</t>
+  </si>
+  <si>
+    <t>416 (59)</t>
+  </si>
+  <si>
+    <t>422 (64)</t>
+  </si>
+  <si>
+    <t>15 (3)</t>
+  </si>
+  <si>
+    <t>16 (3)</t>
+  </si>
+  <si>
+    <t>259 (41)</t>
+  </si>
+  <si>
+    <t>263 (39)</t>
+  </si>
+  <si>
+    <t>48 (12)</t>
+  </si>
+  <si>
+    <t>47 (12)</t>
+  </si>
+  <si>
+    <t>29 (5)</t>
+  </si>
+  <si>
+    <t>30 (4)</t>
+  </si>
+  <si>
+    <t>56 (11)</t>
+  </si>
+  <si>
+    <t>59 (13)</t>
+  </si>
+  <si>
+    <t>34 (7)</t>
+  </si>
+  <si>
+    <t>35 (6)</t>
+  </si>
+  <si>
+    <t>38 (5)</t>
+  </si>
+  <si>
+    <t>39 (4)</t>
+  </si>
+  <si>
+    <t>13 (1)</t>
+  </si>
+  <si>
+    <t>13 (2)</t>
+  </si>
+  <si>
+    <t>Sacrum</t>
+  </si>
+  <si>
+    <t>Hip_R</t>
+  </si>
+  <si>
+    <t>Hip_L</t>
+  </si>
+  <si>
+    <t>Femur_R</t>
+  </si>
+  <si>
+    <t>Femur_L</t>
+  </si>
+  <si>
+    <t>Patella_R</t>
+  </si>
+  <si>
+    <t>Patella_L</t>
+  </si>
+  <si>
+    <t>Tibia_R</t>
+  </si>
+  <si>
+    <t>Tibia_L</t>
+  </si>
+  <si>
+    <t>Fibula_R</t>
+  </si>
+  <si>
+    <t>Fibula_L</t>
+  </si>
+  <si>
+    <t>Talus_R</t>
+  </si>
+  <si>
+    <t>Talus_L</t>
+  </si>
+  <si>
+    <t>Calcaneus_R</t>
+  </si>
+  <si>
+    <t>Calcaneus_L</t>
+  </si>
+  <si>
+    <t>Tarsals_R</t>
+  </si>
+  <si>
+    <t>Tarsals_L</t>
+  </si>
+  <si>
+    <t>Metatarsals_R</t>
+  </si>
+  <si>
+    <t>Metatarsals_L</t>
+  </si>
+  <si>
+    <t>Phalanges_R</t>
+  </si>
+  <si>
+    <t>Phalanges_L</t>
+  </si>
+  <si>
+    <t>203 ± 27</t>
+  </si>
+  <si>
+    <t>327 ± 56</t>
+  </si>
+  <si>
+    <t>328 ± 55</t>
+  </si>
+  <si>
+    <t>531 ± 113</t>
+  </si>
+  <si>
+    <t>533 ± 113</t>
+  </si>
+  <si>
+    <t>19 ± 5</t>
+  </si>
+  <si>
+    <t>333 ± 74</t>
+  </si>
+  <si>
+    <t>336 ± 73</t>
+  </si>
+  <si>
+    <t>61 ± 16</t>
+  </si>
+  <si>
+    <t>60 ± 15</t>
+  </si>
+  <si>
+    <t>37 ± 9</t>
+  </si>
+  <si>
+    <t>38 ± 9</t>
+  </si>
+  <si>
+    <t>70 ± 14</t>
+  </si>
+  <si>
+    <t>43 ± 9</t>
+  </si>
+  <si>
+    <t>43 ± 10</t>
+  </si>
+  <si>
+    <t>48 ± 10</t>
+  </si>
+  <si>
+    <t>48 ± 9</t>
+  </si>
+  <si>
+    <t>15 ± 3</t>
+  </si>
+  <si>
+    <t>198 (35)</t>
+  </si>
+  <si>
+    <t>312 (90)</t>
+  </si>
+  <si>
+    <t>313 (91)</t>
+  </si>
+  <si>
+    <t>542 (214)</t>
+  </si>
+  <si>
+    <t>545 (209)</t>
+  </si>
+  <si>
+    <t>19 (7)</t>
+  </si>
+  <si>
+    <t>352 (135)</t>
+  </si>
+  <si>
+    <t>353 (139)</t>
+  </si>
+  <si>
+    <t>62 (21)</t>
+  </si>
+  <si>
+    <t>59 (20)</t>
+  </si>
+  <si>
+    <t>35 (17)</t>
+  </si>
+  <si>
+    <t>35 (16)</t>
+  </si>
+  <si>
+    <t>68 (24)</t>
+  </si>
+  <si>
+    <t>69 (22)</t>
+  </si>
+  <si>
+    <t>43 (16)</t>
+  </si>
+  <si>
+    <t>43 (17)</t>
+  </si>
+  <si>
+    <t>47 (17)</t>
+  </si>
+  <si>
+    <t>15 (5)</t>
+  </si>
+  <si>
+    <t>15 (4)</t>
+  </si>
+  <si>
+    <t>208 ± 27</t>
+  </si>
+  <si>
+    <t>365 ± 52</t>
+  </si>
+  <si>
+    <t>364 ± 50</t>
+  </si>
+  <si>
+    <t>624 ± 66</t>
+  </si>
+  <si>
+    <t>630 ± 57</t>
+  </si>
+  <si>
+    <t>23 ± 4</t>
+  </si>
+  <si>
+    <t>395 ± 39</t>
+  </si>
+  <si>
+    <t>398 ± 35</t>
+  </si>
+  <si>
+    <t>73 ± 12</t>
+  </si>
+  <si>
+    <t>70 ± 13</t>
+  </si>
+  <si>
+    <t>44 ± 6</t>
+  </si>
+  <si>
+    <t>80 ± 11</t>
+  </si>
+  <si>
+    <t>80 ± 10</t>
+  </si>
+  <si>
+    <t>50 ± 6</t>
+  </si>
+  <si>
+    <t>56 ± 6</t>
+  </si>
+  <si>
+    <t>56 ± 5</t>
+  </si>
+  <si>
+    <t>18 ± 3</t>
+  </si>
+  <si>
+    <t>215 (42)</t>
+  </si>
+  <si>
+    <t>382 (83)</t>
+  </si>
+  <si>
+    <t>381 (81)</t>
+  </si>
+  <si>
+    <t>630 (94)</t>
+  </si>
+  <si>
+    <t>631 (47)</t>
+  </si>
+  <si>
+    <t>21 (6)</t>
+  </si>
+  <si>
+    <t>22 (4)</t>
+  </si>
+  <si>
+    <t>394 (47)</t>
+  </si>
+  <si>
+    <t>402 (32)</t>
+  </si>
+  <si>
+    <t>69 (13)</t>
+  </si>
+  <si>
+    <t>66 (10)</t>
+  </si>
+  <si>
+    <t>46 (9)</t>
+  </si>
+  <si>
+    <t>44 (5)</t>
+  </si>
+  <si>
+    <t>80 (7)</t>
+  </si>
+  <si>
+    <t>81 (8)</t>
+  </si>
+  <si>
+    <t>49 (9)</t>
+  </si>
+  <si>
+    <t>50 (8)</t>
+  </si>
+  <si>
+    <t>56 (5)</t>
+  </si>
+  <si>
+    <t>55 (3)</t>
+  </si>
+  <si>
+    <t>17 (3)</t>
+  </si>
+  <si>
+    <t>17 (2)</t>
+  </si>
+  <si>
+    <t>198 ± 27</t>
+  </si>
+  <si>
+    <t>290 ± 28</t>
+  </si>
+  <si>
+    <t>292 ± 31</t>
+  </si>
+  <si>
+    <t>437 ± 56</t>
+  </si>
+  <si>
+    <t>436 ± 55</t>
+  </si>
+  <si>
+    <t>15 ± 2</t>
+  </si>
+  <si>
+    <t>15 ± 3</t>
+  </si>
+  <si>
+    <t>270 ± 37</t>
+  </si>
+  <si>
+    <t>274 ± 38</t>
+  </si>
+  <si>
+    <t>50 ± 8</t>
+  </si>
+  <si>
+    <t>50 ± 9</t>
+  </si>
+  <si>
+    <t>30 ± 5</t>
+  </si>
+  <si>
+    <t>31 ± 6</t>
+  </si>
+  <si>
+    <t>59 ± 8</t>
+  </si>
+  <si>
+    <t>59 ± 9</t>
+  </si>
+  <si>
+    <t>36 ± 6</t>
+  </si>
+  <si>
+    <t>36 ± 7</t>
+  </si>
+  <si>
+    <t>40 ± 4</t>
+  </si>
+  <si>
+    <t>13 ± 1</t>
+  </si>
+  <si>
+    <t>193 (29)</t>
+  </si>
+  <si>
+    <t>292 (39)</t>
+  </si>
+  <si>
+    <t>290 (50)</t>
+  </si>
+  <si>
+    <t>416 (59)</t>
+  </si>
+  <si>
+    <t>422 (64)</t>
+  </si>
+  <si>
+    <t>15 (3)</t>
+  </si>
+  <si>
+    <t>16 (3)</t>
+  </si>
+  <si>
+    <t>259 (41)</t>
+  </si>
+  <si>
+    <t>263 (39)</t>
+  </si>
+  <si>
+    <t>48 (12)</t>
+  </si>
+  <si>
+    <t>47 (12)</t>
+  </si>
+  <si>
+    <t>29 (5)</t>
+  </si>
+  <si>
+    <t>30 (4)</t>
+  </si>
+  <si>
+    <t>56 (11)</t>
+  </si>
+  <si>
+    <t>59 (13)</t>
+  </si>
+  <si>
+    <t>34 (7)</t>
+  </si>
+  <si>
+    <t>35 (6)</t>
+  </si>
+  <si>
+    <t>38 (5)</t>
+  </si>
+  <si>
+    <t>39 (4)</t>
+  </si>
+  <si>
+    <t>13 (1)</t>
+  </si>
+  <si>
+    <t>13 (2)</t>
+  </si>
+  <si>
+    <t>Sacrum</t>
+  </si>
+  <si>
+    <t>Hip_R</t>
+  </si>
+  <si>
+    <t>Hip_L</t>
+  </si>
+  <si>
+    <t>Femur_R</t>
+  </si>
+  <si>
+    <t>Femur_L</t>
+  </si>
+  <si>
+    <t>Patella_R</t>
+  </si>
+  <si>
+    <t>Patella_L</t>
+  </si>
+  <si>
+    <t>Tibia_R</t>
+  </si>
+  <si>
+    <t>Tibia_L</t>
+  </si>
+  <si>
+    <t>Fibula_R</t>
+  </si>
+  <si>
+    <t>Fibula_L</t>
+  </si>
+  <si>
+    <t>Talus_R</t>
+  </si>
+  <si>
+    <t>Talus_L</t>
+  </si>
+  <si>
+    <t>Calcaneus_R</t>
+  </si>
+  <si>
+    <t>Calcaneus_L</t>
+  </si>
+  <si>
+    <t>Tarsals_R</t>
+  </si>
+  <si>
+    <t>Tarsals_L</t>
+  </si>
+  <si>
+    <t>Metatarsals_R</t>
+  </si>
+  <si>
+    <t>Metatarsals_L</t>
+  </si>
+  <si>
+    <t>Phalanges_R</t>
+  </si>
+  <si>
+    <t>Phalanges_L</t>
+  </si>
+  <si>
+    <t>203 ± 27</t>
+  </si>
+  <si>
+    <t>327 ± 56</t>
+  </si>
+  <si>
+    <t>328 ± 55</t>
+  </si>
+  <si>
+    <t>531 ± 113</t>
+  </si>
+  <si>
+    <t>533 ± 113</t>
+  </si>
+  <si>
+    <t>19 ± 5</t>
+  </si>
+  <si>
+    <t>333 ± 74</t>
+  </si>
+  <si>
+    <t>336 ± 73</t>
+  </si>
+  <si>
+    <t>61 ± 16</t>
+  </si>
+  <si>
+    <t>60 ± 15</t>
+  </si>
+  <si>
+    <t>37 ± 9</t>
+  </si>
+  <si>
+    <t>38 ± 9</t>
+  </si>
+  <si>
+    <t>70 ± 14</t>
+  </si>
+  <si>
+    <t>43 ± 9</t>
+  </si>
+  <si>
+    <t>43 ± 10</t>
+  </si>
+  <si>
+    <t>48 ± 10</t>
+  </si>
+  <si>
+    <t>48 ± 9</t>
+  </si>
+  <si>
+    <t>15 ± 3</t>
+  </si>
+  <si>
+    <t>198 (35)</t>
+  </si>
+  <si>
+    <t>312 (90)</t>
+  </si>
+  <si>
+    <t>313 (91)</t>
+  </si>
+  <si>
+    <t>542 (214)</t>
+  </si>
+  <si>
+    <t>545 (209)</t>
+  </si>
+  <si>
+    <t>19 (7)</t>
+  </si>
+  <si>
+    <t>352 (135)</t>
+  </si>
+  <si>
+    <t>353 (139)</t>
+  </si>
+  <si>
+    <t>62 (21)</t>
+  </si>
+  <si>
+    <t>59 (20)</t>
+  </si>
+  <si>
+    <t>35 (17)</t>
+  </si>
+  <si>
+    <t>35 (16)</t>
+  </si>
+  <si>
+    <t>68 (24)</t>
+  </si>
+  <si>
+    <t>69 (22)</t>
+  </si>
+  <si>
+    <t>43 (16)</t>
+  </si>
+  <si>
+    <t>43 (17)</t>
+  </si>
+  <si>
+    <t>47 (17)</t>
+  </si>
+  <si>
+    <t>15 (5)</t>
+  </si>
+  <si>
+    <t>15 (4)</t>
+  </si>
+  <si>
+    <t>208 ± 27</t>
+  </si>
+  <si>
+    <t>365 ± 52</t>
+  </si>
+  <si>
+    <t>364 ± 50</t>
+  </si>
+  <si>
+    <t>624 ± 66</t>
+  </si>
+  <si>
+    <t>630 ± 57</t>
+  </si>
+  <si>
+    <t>23 ± 4</t>
+  </si>
+  <si>
+    <t>395 ± 39</t>
+  </si>
+  <si>
+    <t>398 ± 35</t>
+  </si>
+  <si>
+    <t>73 ± 12</t>
+  </si>
+  <si>
+    <t>70 ± 13</t>
+  </si>
+  <si>
+    <t>44 ± 6</t>
+  </si>
+  <si>
+    <t>80 ± 11</t>
+  </si>
+  <si>
+    <t>80 ± 10</t>
+  </si>
+  <si>
+    <t>50 ± 6</t>
+  </si>
+  <si>
+    <t>56 ± 6</t>
+  </si>
+  <si>
+    <t>56 ± 5</t>
+  </si>
+  <si>
+    <t>18 ± 3</t>
+  </si>
+  <si>
+    <t>215 (42)</t>
+  </si>
+  <si>
+    <t>382 (83)</t>
+  </si>
+  <si>
+    <t>381 (81)</t>
+  </si>
+  <si>
+    <t>630 (94)</t>
+  </si>
+  <si>
+    <t>631 (47)</t>
+  </si>
+  <si>
+    <t>21 (6)</t>
+  </si>
+  <si>
+    <t>22 (4)</t>
+  </si>
+  <si>
+    <t>394 (47)</t>
+  </si>
+  <si>
+    <t>402 (32)</t>
+  </si>
+  <si>
+    <t>69 (13)</t>
+  </si>
+  <si>
+    <t>66 (10)</t>
+  </si>
+  <si>
+    <t>46 (9)</t>
+  </si>
+  <si>
+    <t>44 (5)</t>
+  </si>
+  <si>
+    <t>80 (7)</t>
+  </si>
+  <si>
+    <t>81 (8)</t>
+  </si>
+  <si>
+    <t>49 (9)</t>
+  </si>
+  <si>
+    <t>50 (8)</t>
+  </si>
+  <si>
+    <t>56 (5)</t>
+  </si>
+  <si>
+    <t>55 (3)</t>
+  </si>
+  <si>
+    <t>17 (3)</t>
+  </si>
+  <si>
+    <t>17 (2)</t>
+  </si>
+  <si>
+    <t>198 ± 27</t>
+  </si>
+  <si>
+    <t>290 ± 28</t>
+  </si>
+  <si>
+    <t>292 ± 31</t>
+  </si>
+  <si>
+    <t>437 ± 56</t>
+  </si>
+  <si>
+    <t>436 ± 55</t>
+  </si>
+  <si>
+    <t>15 ± 2</t>
+  </si>
+  <si>
+    <t>15 ± 3</t>
+  </si>
+  <si>
+    <t>270 ± 37</t>
+  </si>
+  <si>
+    <t>274 ± 38</t>
+  </si>
+  <si>
+    <t>50 ± 8</t>
+  </si>
+  <si>
+    <t>50 ± 9</t>
+  </si>
+  <si>
+    <t>30 ± 5</t>
+  </si>
+  <si>
+    <t>31 ± 6</t>
+  </si>
+  <si>
+    <t>59 ± 8</t>
+  </si>
+  <si>
+    <t>59 ± 9</t>
+  </si>
+  <si>
+    <t>36 ± 6</t>
+  </si>
+  <si>
+    <t>36 ± 7</t>
+  </si>
+  <si>
+    <t>40 ± 4</t>
+  </si>
+  <si>
+    <t>13 ± 1</t>
+  </si>
+  <si>
+    <t>193 (29)</t>
+  </si>
+  <si>
+    <t>292 (39)</t>
+  </si>
+  <si>
+    <t>290 (50)</t>
+  </si>
+  <si>
+    <t>416 (59)</t>
+  </si>
+  <si>
+    <t>422 (64)</t>
+  </si>
+  <si>
+    <t>15 (3)</t>
+  </si>
+  <si>
+    <t>16 (3)</t>
+  </si>
+  <si>
+    <t>259 (41)</t>
+  </si>
+  <si>
+    <t>263 (39)</t>
+  </si>
+  <si>
+    <t>48 (12)</t>
+  </si>
+  <si>
+    <t>47 (12)</t>
+  </si>
+  <si>
+    <t>29 (5)</t>
+  </si>
+  <si>
+    <t>30 (4)</t>
+  </si>
+  <si>
+    <t>56 (11)</t>
+  </si>
+  <si>
+    <t>59 (13)</t>
+  </si>
+  <si>
+    <t>34 (7)</t>
+  </si>
+  <si>
+    <t>35 (6)</t>
+  </si>
+  <si>
+    <t>38 (5)</t>
   </si>
   <si>
     <t>39 (4)</t>
@@ -478,7 +2926,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -678,65 +3126,67 @@
       </bottom>
       <diagonal/>
     </border>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1053,28 +3503,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:N25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="false" tabSelected="true" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" customWidth="1"/>
-    <col min="3" max="3" width="5.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3" customWidth="true"/>
+    <col min="2" max="2" width="13.5703125" customWidth="true"/>
+    <col min="3" max="3" width="4.140625" style="3" bestFit="true" customWidth="true"/>
+    <col min="4" max="4" width="9" bestFit="true" customWidth="true"/>
+    <col min="5" max="5" width="9" bestFit="true" customWidth="true"/>
+    <col min="6" max="6" width="4.140625" style="3" bestFit="true" customWidth="true"/>
+    <col min="7" max="7" width="4.140625" bestFit="true" customWidth="true"/>
+    <col min="8" max="8" width="8" bestFit="true" customWidth="true"/>
+    <col min="9" max="9" width="8" bestFit="true" customWidth="true"/>
+    <col min="10" max="10" width="4.140625" bestFit="true" customWidth="true"/>
+    <col min="11" max="11" width="4.140625" bestFit="true" customWidth="true"/>
+    <col min="12" max="12" width="8" bestFit="true" customWidth="true"/>
+    <col min="13" max="13" width="8" bestFit="true" customWidth="true"/>
+    <col min="14" max="14" width="4.140625" bestFit="true" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" ht="15.75" thickBot="1"/>
-    <row r="2" spans="2:14" ht="15.75" thickBot="1">
+    <row r="1" ht="15.75" thickBot="true"/>
+    <row r="2" ht="15.75" thickBot="true">
       <c r="C2" s="17" t="s">
         <v>5</v>
       </c>
@@ -1090,7 +3540,7 @@
       <c r="M2" s="18"/>
       <c r="N2" s="19"/>
     </row>
-    <row r="3" spans="2:14">
+    <row r="3">
       <c r="B3" s="4"/>
       <c r="C3" s="14" t="s">
         <v>8</v>
@@ -1111,7 +3561,7 @@
       <c r="M3" s="15"/>
       <c r="N3" s="16"/>
     </row>
-    <row r="4" spans="2:14">
+    <row r="4">
       <c r="B4" s="5" t="s">
         <v>0</v>
       </c>
@@ -1152,865 +3602,865 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:14">
+    <row r="5">
       <c r="B5" s="6" t="s">
-        <v>9</v>
+        <v>824</v>
       </c>
       <c r="C5" s="9">
-        <v>159.01177934791318</v>
+        <v>158.63963711809413</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>30</v>
+        <v>845</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>48</v>
+        <v>863</v>
       </c>
       <c r="F5" s="10">
-        <v>257.68767348504866</v>
+        <v>257.1775384374331</v>
       </c>
       <c r="G5" s="9">
-        <v>159.01177934791318</v>
+        <v>158.63963711809413</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>66</v>
+        <v>882</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>84</v>
+        <v>899</v>
       </c>
       <c r="J5" s="10">
-        <v>242.2973707233366</v>
+        <v>242.03020400273181</v>
       </c>
       <c r="K5" s="9">
-        <v>159.03429644135798</v>
+        <v>158.68834162590244</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>105</v>
+        <v>920</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>124</v>
+        <v>939</v>
       </c>
       <c r="N5" s="10">
-        <v>257.68767348504866</v>
+        <v>257.1775384374331</v>
       </c>
     </row>
-    <row r="6" spans="2:14">
+    <row r="6">
       <c r="B6" s="6" t="s">
-        <v>10</v>
+        <v>825</v>
       </c>
       <c r="C6" s="9">
-        <v>255.60664497125507</v>
+        <v>255.18479003655801</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>31</v>
+        <v>846</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>49</v>
+        <v>864</v>
       </c>
       <c r="F6" s="10">
-        <v>453.54094605697799</v>
+        <v>452.84443173140636</v>
       </c>
       <c r="G6" s="9">
-        <v>299.22788852956739</v>
+        <v>298.69537368364962</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>67</v>
+        <v>883</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>85</v>
+        <v>900</v>
       </c>
       <c r="J6" s="10">
-        <v>453.54094605697799</v>
+        <v>452.84443173140636</v>
       </c>
       <c r="K6" s="9">
-        <v>255.60664497125507</v>
+        <v>255.18479003655801</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>106</v>
+        <v>921</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>125</v>
+        <v>940</v>
       </c>
       <c r="N6" s="10">
-        <v>339.80516491961083</v>
+        <v>339.17280188266045</v>
       </c>
     </row>
-    <row r="7" spans="2:14">
+    <row r="7">
       <c r="B7" s="6" t="s">
-        <v>11</v>
+        <v>826</v>
       </c>
       <c r="C7" s="9">
-        <v>239.3154822239201</v>
+        <v>238.86147553204341</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>32</v>
+        <v>847</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>50</v>
+        <v>865</v>
       </c>
       <c r="F7" s="10">
-        <v>447.99064899131992</v>
+        <v>447.23495504296989</v>
       </c>
       <c r="G7" s="9">
-        <v>299.20997954111704</v>
+        <v>298.81739719516827</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>68</v>
+        <v>884</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>86</v>
+        <v>901</v>
       </c>
       <c r="J7" s="10">
-        <v>447.99064899131992</v>
+        <v>447.23495504296989</v>
       </c>
       <c r="K7" s="9">
-        <v>239.3154822239201</v>
+        <v>238.86147553204341</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>107</v>
+        <v>922</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>126</v>
+        <v>941</v>
       </c>
       <c r="N7" s="10">
-        <v>335.68835104083661</v>
+        <v>335.15153310203823</v>
       </c>
     </row>
-    <row r="8" spans="2:14">
+    <row r="8">
       <c r="B8" s="6" t="s">
-        <v>12</v>
+        <v>827</v>
       </c>
       <c r="C8" s="9">
-        <v>382.15101397977611</v>
+        <v>380.2053142162261</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>33</v>
+        <v>848</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>51</v>
+        <v>866</v>
       </c>
       <c r="F8" s="10">
-        <v>771.60648733335051</v>
+        <v>768.33912275198747</v>
       </c>
       <c r="G8" s="9">
-        <v>549.83117157702077</v>
+        <v>547.06567233031296</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>69</v>
+        <v>885</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>87</v>
+        <v>902</v>
       </c>
       <c r="J8" s="10">
-        <v>771.60648733335051</v>
+        <v>768.33912275198747</v>
       </c>
       <c r="K8" s="9">
-        <v>382.15101397977611</v>
+        <v>380.2053142162261</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>108</v>
+        <v>923</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>127</v>
+        <v>942</v>
       </c>
       <c r="N8" s="10">
-        <v>539.93979312141653</v>
+        <v>537.26402634968201</v>
       </c>
     </row>
-    <row r="9" spans="2:14">
+    <row r="9">
       <c r="B9" s="6" t="s">
-        <v>13</v>
+        <v>828</v>
       </c>
       <c r="C9" s="9">
-        <v>368.79522084447211</v>
+        <v>366.92676653362457</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>34</v>
+        <v>849</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>52</v>
+        <v>867</v>
       </c>
       <c r="F9" s="10">
-        <v>761.54801560776104</v>
+        <v>758.34897282963402</v>
       </c>
       <c r="G9" s="9">
-        <v>556.18238320310309</v>
+        <v>553.81646021238657</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>70</v>
+        <v>886</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>88</v>
+        <v>903</v>
       </c>
       <c r="J9" s="10">
-        <v>761.54801560776104</v>
+        <v>758.34897282963402</v>
       </c>
       <c r="K9" s="9">
-        <v>368.79522084447211</v>
+        <v>366.92676653362457</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>109</v>
+        <v>924</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>128</v>
+        <v>943</v>
       </c>
       <c r="N9" s="10">
-        <v>538.34017087354471</v>
+        <v>535.69855548830844</v>
       </c>
     </row>
-    <row r="10" spans="2:14">
+    <row r="10">
       <c r="B10" s="6" t="s">
-        <v>14</v>
+        <v>829</v>
       </c>
       <c r="C10" s="9">
-        <v>11.060730933244383</v>
+        <v>10.946596173874976</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>35</v>
+        <v>850</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>53</v>
+        <v>868</v>
       </c>
       <c r="F10" s="10">
-        <v>30.678709510213743</v>
+        <v>30.490503578909319</v>
       </c>
       <c r="G10" s="9">
-        <v>19.278053672711657</v>
+        <v>19.116694885379619</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>71</v>
+        <v>887</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>89</v>
+        <v>904</v>
       </c>
       <c r="J10" s="10">
-        <v>30.678709510213743</v>
+        <v>30.490503578909319</v>
       </c>
       <c r="K10" s="9">
-        <v>11.060730933244383</v>
+        <v>10.946596173874976</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>110</v>
+        <v>925</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>129</v>
+        <v>944</v>
       </c>
       <c r="N10" s="10">
-        <v>18.403927492331452</v>
+        <v>18.217605077472133</v>
       </c>
     </row>
-    <row r="11" spans="2:14">
+    <row r="11">
       <c r="B11" s="6" t="s">
-        <v>15</v>
+        <v>830</v>
       </c>
       <c r="C11" s="9">
-        <v>11.60585804057674</v>
+        <v>11.472058731846028</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>35</v>
+        <v>850</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>53</v>
+        <v>868</v>
       </c>
       <c r="F11" s="10">
-        <v>31.670808305195486</v>
+        <v>31.484334959892045</v>
       </c>
       <c r="G11" s="9">
-        <v>18.812267884199336</v>
+        <v>18.666194067996624</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>71</v>
+        <v>887</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>90</v>
+        <v>905</v>
       </c>
       <c r="J11" s="10">
-        <v>31.670808305195486</v>
+        <v>31.484334959892045</v>
       </c>
       <c r="K11" s="9">
-        <v>11.60585804057674</v>
+        <v>11.472058731846028</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>111</v>
+        <v>926</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>130</v>
+        <v>945</v>
       </c>
       <c r="N11" s="10">
-        <v>19.815004366248999</v>
+        <v>19.628212925832678</v>
       </c>
     </row>
-    <row r="12" spans="2:14">
+    <row r="12">
       <c r="B12" s="6" t="s">
-        <v>16</v>
+        <v>831</v>
       </c>
       <c r="C12" s="9">
-        <v>235.33417757902004</v>
+        <v>234.22207032868826</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>36</v>
+        <v>851</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>54</v>
+        <v>869</v>
       </c>
       <c r="F12" s="10">
-        <v>483.66647554695999</v>
+        <v>481.85569190058828</v>
       </c>
       <c r="G12" s="9">
-        <v>355.33293641496198</v>
+        <v>354.20763570767491</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>72</v>
+        <v>888</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>91</v>
+        <v>906</v>
       </c>
       <c r="J12" s="10">
-        <v>483.66647554695999</v>
+        <v>481.85569190058828</v>
       </c>
       <c r="K12" s="9">
-        <v>235.33417757902004</v>
+        <v>234.22207032868826</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>112</v>
+        <v>927</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>131</v>
+        <v>946</v>
       </c>
       <c r="N12" s="10">
-        <v>351.87930547056237</v>
+        <v>350.35230291845352</v>
       </c>
     </row>
-    <row r="13" spans="2:14">
+    <row r="13">
       <c r="B13" s="6" t="s">
-        <v>17</v>
+        <v>832</v>
       </c>
       <c r="C13" s="9">
-        <v>237.14294606781442</v>
+        <v>235.91142489319543</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>37</v>
+        <v>852</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>55</v>
+        <v>870</v>
       </c>
       <c r="F13" s="10">
-        <v>478.55181549202115</v>
+        <v>476.8509307970167</v>
       </c>
       <c r="G13" s="9">
-        <v>353.21956783022921</v>
+        <v>351.78355856690064</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>73</v>
+        <v>889</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>92</v>
+        <v>907</v>
       </c>
       <c r="J13" s="10">
-        <v>478.55181549202115</v>
+        <v>476.8509307970167</v>
       </c>
       <c r="K13" s="9">
-        <v>237.14294606781442</v>
+        <v>235.91142489319543</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>113</v>
+        <v>928</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>132</v>
+        <v>947</v>
       </c>
       <c r="N13" s="10">
-        <v>357.91248357161743</v>
+        <v>356.41873127923446</v>
       </c>
     </row>
-    <row r="14" spans="2:14">
+    <row r="14">
       <c r="B14" s="6" t="s">
-        <v>18</v>
+        <v>833</v>
       </c>
       <c r="C14" s="9">
-        <v>40.007581978338273</v>
+        <v>39.531811739229127</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>38</v>
+        <v>853</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>56</v>
+        <v>871</v>
       </c>
       <c r="F14" s="10">
-        <v>103.86094898534905</v>
+        <v>102.9324227483377</v>
       </c>
       <c r="G14" s="9">
-        <v>61.526519028456256</v>
+        <v>60.817716410020729</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>74</v>
+        <v>890</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>93</v>
+        <v>908</v>
       </c>
       <c r="J14" s="10">
-        <v>103.86094898534905</v>
+        <v>102.9324227483377</v>
       </c>
       <c r="K14" s="9">
-        <v>40.007581978338273</v>
+        <v>39.531811739229127</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>114</v>
+        <v>929</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>133</v>
+        <v>948</v>
       </c>
       <c r="N14" s="10">
-        <v>65.666254633351897</v>
+        <v>65.01630673696495</v>
       </c>
     </row>
-    <row r="15" spans="2:14">
+    <row r="15">
       <c r="B15" s="6" t="s">
-        <v>19</v>
+        <v>834</v>
       </c>
       <c r="C15" s="9">
-        <v>37.561089633043089</v>
+        <v>37.055272261158883</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>39</v>
+        <v>854</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>57</v>
+        <v>872</v>
       </c>
       <c r="F15" s="10">
-        <v>103.71304122731408</v>
+        <v>102.83415315792166</v>
       </c>
       <c r="G15" s="9">
-        <v>59.238490529110379</v>
+        <v>58.660870345964057</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>75</v>
+        <v>891</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>94</v>
+        <v>909</v>
       </c>
       <c r="J15" s="10">
-        <v>103.71304122731408</v>
+        <v>102.83415315792166</v>
       </c>
       <c r="K15" s="9">
-        <v>37.561089633043089</v>
+        <v>37.055272261158883</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>115</v>
+        <v>930</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>133</v>
+        <v>949</v>
       </c>
       <c r="N15" s="10">
-        <v>68.222557874019287</v>
+        <v>67.503321430144609</v>
       </c>
     </row>
-    <row r="16" spans="2:14">
+    <row r="16">
       <c r="B16" s="6" t="s">
-        <v>20</v>
+        <v>835</v>
       </c>
       <c r="C16" s="9">
-        <v>25.805285313618253</v>
+        <v>25.625356311992736</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>40</v>
+        <v>855</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>58</v>
+        <v>873</v>
       </c>
       <c r="F16" s="10">
-        <v>53.546388528150082</v>
+        <v>53.26195439342829</v>
       </c>
       <c r="G16" s="9">
-        <v>35.343414810190005</v>
+        <v>35.126819575076262</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>76</v>
+        <v>892</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>95</v>
+        <v>910</v>
       </c>
       <c r="J16" s="10">
-        <v>53.546388528150082</v>
+        <v>53.26195439342829</v>
       </c>
       <c r="K16" s="9">
-        <v>25.805285313618253</v>
+        <v>25.625356311992736</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>116</v>
+        <v>931</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>134</v>
+        <v>950</v>
       </c>
       <c r="N16" s="10">
-        <v>43.269160433846963</v>
+        <v>42.999105014618472</v>
       </c>
     </row>
-    <row r="17" spans="2:14">
+    <row r="17">
       <c r="B17" s="6" t="s">
-        <v>21</v>
+        <v>836</v>
       </c>
       <c r="C17" s="9">
-        <v>25.16564147078164</v>
+        <v>24.967871513242578</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>41</v>
+        <v>856</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>59</v>
+        <v>874</v>
       </c>
       <c r="F17" s="10">
-        <v>54.154087978341465</v>
+        <v>53.861909486387674</v>
       </c>
       <c r="G17" s="9">
-        <v>34.561722037893453</v>
+        <v>34.365198864052154</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>77</v>
+        <v>892</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>96</v>
+        <v>911</v>
       </c>
       <c r="J17" s="10">
-        <v>54.154087978341465</v>
+        <v>53.861909486387674</v>
       </c>
       <c r="K17" s="9">
-        <v>25.16564147078164</v>
+        <v>24.967871513242578</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>117</v>
+        <v>932</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>135</v>
+        <v>951</v>
       </c>
       <c r="N17" s="10">
-        <v>46.824310416893105</v>
+        <v>46.60930605961817</v>
       </c>
     </row>
-    <row r="18" spans="2:14">
+    <row r="18">
       <c r="B18" s="6" t="s">
-        <v>22</v>
+        <v>837</v>
       </c>
       <c r="C18" s="9">
-        <v>51.285536979511924</v>
+        <v>51.024561755368694</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>42</v>
+        <v>857</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>60</v>
+        <v>875</v>
       </c>
       <c r="F18" s="10">
-        <v>102.29816942794594</v>
+        <v>101.88938781076911</v>
       </c>
       <c r="G18" s="9">
-        <v>61.782435681198983</v>
+        <v>61.527750399233454</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>78</v>
+        <v>893</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>97</v>
+        <v>912</v>
       </c>
       <c r="J18" s="10">
-        <v>102.29816942794594</v>
+        <v>101.88938781076911</v>
       </c>
       <c r="K18" s="9">
-        <v>51.285536979511924</v>
+        <v>51.024561755368694</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>118</v>
+        <v>933</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>136</v>
+        <v>952</v>
       </c>
       <c r="N18" s="10">
-        <v>77.888873780489178</v>
+        <v>77.519373785076255</v>
       </c>
     </row>
-    <row r="19" spans="2:14">
+    <row r="19">
       <c r="B19" s="6" t="s">
-        <v>23</v>
+        <v>838</v>
       </c>
       <c r="C19" s="9">
-        <v>49.467830056926203</v>
+        <v>49.234557887543865</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>42</v>
+        <v>857</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>61</v>
+        <v>876</v>
       </c>
       <c r="F19" s="10">
-        <v>98.549859594971508</v>
+        <v>98.142943064277645</v>
       </c>
       <c r="G19" s="9">
-        <v>61.938285189972106</v>
+        <v>61.683390969706416</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>79</v>
+        <v>894</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>98</v>
+        <v>913</v>
       </c>
       <c r="J19" s="10">
-        <v>98.549859594971508</v>
+        <v>98.142943064277645</v>
       </c>
       <c r="K19" s="9">
-        <v>49.467830056926203</v>
+        <v>49.234557887543865</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>119</v>
+        <v>934</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>137</v>
+        <v>953</v>
       </c>
       <c r="N19" s="10">
-        <v>77.027093300618134</v>
+        <v>76.666634493468848</v>
       </c>
     </row>
-    <row r="20" spans="2:14">
+    <row r="20">
       <c r="B20" s="6" t="s">
-        <v>24</v>
+        <v>839</v>
       </c>
       <c r="C20" s="9">
-        <v>30.565332696571385</v>
+        <v>30.229385471162946</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>43</v>
+        <v>858</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>62</v>
+        <v>877</v>
       </c>
       <c r="F20" s="10">
-        <v>60.457429993993088</v>
+        <v>59.926994348781776</v>
       </c>
       <c r="G20" s="9">
-        <v>41.756450918328206</v>
+        <v>41.374984134098227</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>80</v>
+        <v>895</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>99</v>
+        <v>914</v>
       </c>
       <c r="J20" s="10">
-        <v>60.457429993993088</v>
+        <v>59.926994348781776</v>
       </c>
       <c r="K20" s="9">
-        <v>30.565332696571385</v>
+        <v>30.229385471162946</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>120</v>
+        <v>935</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>138</v>
+        <v>954</v>
       </c>
       <c r="N20" s="10">
-        <v>49.964787604945187</v>
+        <v>49.489392354601577</v>
       </c>
     </row>
-    <row r="21" spans="2:14">
+    <row r="21">
       <c r="B21" s="6" t="s">
-        <v>25</v>
+        <v>840</v>
       </c>
       <c r="C21" s="9">
-        <v>29.467423949875165</v>
+        <v>29.11944008387395</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>44</v>
+        <v>859</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>63</v>
+        <v>878</v>
       </c>
       <c r="F21" s="10">
-        <v>61.747006010444245</v>
+        <v>61.234290825868243</v>
       </c>
       <c r="G21" s="9">
-        <v>40.347255760962462</v>
+        <v>39.984234922781589</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>80</v>
+        <v>895</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>100</v>
+        <v>915</v>
       </c>
       <c r="J21" s="10">
-        <v>61.747006010444245</v>
+        <v>61.234290825868243</v>
       </c>
       <c r="K21" s="9">
-        <v>29.467423949875165</v>
+        <v>29.11944008387395</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>121</v>
+        <v>936</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>139</v>
+        <v>955</v>
       </c>
       <c r="N21" s="10">
-        <v>51.823795575644809</v>
+        <v>51.330986058980997</v>
       </c>
     </row>
-    <row r="22" spans="2:14">
+    <row r="22">
       <c r="B22" s="6" t="s">
-        <v>26</v>
+        <v>841</v>
       </c>
       <c r="C22" s="9">
-        <v>36.600418315042461</v>
+        <v>35.99330542217659</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>45</v>
+        <v>860</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>64</v>
+        <v>879</v>
       </c>
       <c r="F22" s="10">
-        <v>66.967222987063252</v>
+        <v>66.079097062364369</v>
       </c>
       <c r="G22" s="9">
-        <v>43.652153876551921</v>
+        <v>43.058084904455733</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>81</v>
+        <v>896</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>101</v>
+        <v>916</v>
       </c>
       <c r="J22" s="10">
-        <v>66.967222987063252</v>
+        <v>66.079097062364369</v>
       </c>
       <c r="K22" s="9">
-        <v>36.600418315042461</v>
+        <v>35.99330542217659</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>122</v>
+        <v>937</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>140</v>
+        <v>956</v>
       </c>
       <c r="N22" s="10">
-        <v>50.885634420121612</v>
+        <v>50.133929417106039</v>
       </c>
     </row>
-    <row r="23" spans="2:14">
+    <row r="23">
       <c r="B23" s="6" t="s">
-        <v>27</v>
+        <v>842</v>
       </c>
       <c r="C23" s="9">
-        <v>35.46956144066089</v>
+        <v>34.884107559861818</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>46</v>
+        <v>861</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>64</v>
+        <v>879</v>
       </c>
       <c r="F23" s="10">
-        <v>66.221901559091847</v>
+        <v>65.36400266022153</v>
       </c>
       <c r="G23" s="9">
-        <v>44.401883453259963</v>
+        <v>43.806529084433066</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>82</v>
+        <v>897</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>102</v>
+        <v>917</v>
       </c>
       <c r="J23" s="10">
-        <v>66.221901559091847</v>
+        <v>65.36400266022153</v>
       </c>
       <c r="K23" s="9">
-        <v>35.46956144066089</v>
+        <v>34.884107559861818</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>122</v>
+        <v>937</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>141</v>
+        <v>957</v>
       </c>
       <c r="N23" s="10">
-        <v>50.688618977381225</v>
+        <v>49.939830224012887</v>
       </c>
     </row>
-    <row r="24" spans="2:14">
+    <row r="24">
       <c r="B24" s="6" t="s">
-        <v>28</v>
+        <v>843</v>
       </c>
       <c r="C24" s="9">
-        <v>11.860233735296582</v>
+        <v>11.566559393058773</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>47</v>
+        <v>862</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>65</v>
+        <v>880</v>
       </c>
       <c r="F24" s="10">
-        <v>23.332978675106833</v>
+        <v>22.822700260250603</v>
       </c>
       <c r="G24" s="9">
-        <v>14.433710508642061</v>
+        <v>14.092097084847046</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>83</v>
+        <v>898</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>103</v>
+        <v>918</v>
       </c>
       <c r="J24" s="10">
-        <v>23.332978675106833</v>
+        <v>22.822700260250603</v>
       </c>
       <c r="K24" s="9">
-        <v>11.860233735296582</v>
+        <v>11.566559393058773</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>123</v>
+        <v>938</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>142</v>
+        <v>958</v>
       </c>
       <c r="N24" s="10">
-        <v>15.681451332839655</v>
+        <v>15.313947865638024</v>
       </c>
     </row>
-    <row r="25" spans="2:14" ht="15.75" thickBot="1">
+    <row r="25" ht="15.75" thickBot="true">
       <c r="B25" s="6" t="s">
-        <v>29</v>
+        <v>844</v>
       </c>
       <c r="C25" s="11">
-        <v>12.321695293798841</v>
+        <v>12.004882291008633</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>47</v>
+        <v>862</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>65</v>
+        <v>881</v>
       </c>
       <c r="F25" s="13">
-        <v>24.521566688053426</v>
+        <v>23.987624399144675</v>
       </c>
       <c r="G25" s="11">
-        <v>13.456182260323526</v>
+        <v>13.132635427572755</v>
       </c>
       <c r="H25" s="12" t="s">
-        <v>83</v>
+        <v>898</v>
       </c>
       <c r="I25" s="12" t="s">
-        <v>104</v>
+        <v>919</v>
       </c>
       <c r="J25" s="13">
-        <v>24.521566688053426</v>
+        <v>23.987624399144675</v>
       </c>
       <c r="K25" s="11">
-        <v>12.321695293798841</v>
+        <v>12.004882291008633</v>
       </c>
       <c r="L25" s="12" t="s">
-        <v>123</v>
+        <v>938</v>
       </c>
       <c r="M25" s="12" t="s">
-        <v>143</v>
+        <v>959</v>
       </c>
       <c r="N25" s="13">
-        <v>15.844565925741248</v>
+        <v>15.473117119784217</v>
       </c>
     </row>
   </sheetData>

</xml_diff>